<commit_message>
changes to variable definitions for version1.50
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.43.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.43.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1231,18 +1231,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1541,12 +1541,12 @@
     <col min="2" max="3" width="79" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="33" customFormat="1" ht="20.25" thickBot="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:3" s="30" customFormat="1" ht="20.25" thickBot="1">
+      <c r="A1" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1"/>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
@@ -2068,7 +2068,7 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="32" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       <c r="B67" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="31"/>
+      <c r="C67" s="33"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
@@ -2088,7 +2088,7 @@
       <c r="B68" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="31"/>
+      <c r="C68" s="33"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
@@ -2097,7 +2097,7 @@
       <c r="B69" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="31"/>
+      <c r="C69" s="33"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
@@ -2106,7 +2106,7 @@
       <c r="B70" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C70" s="31"/>
+      <c r="C70" s="33"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
@@ -2115,7 +2115,7 @@
       <c r="B71" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="31"/>
+      <c r="C71" s="33"/>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
@@ -2124,7 +2124,7 @@
       <c r="B72" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="31"/>
+      <c r="C72" s="33"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
@@ -2133,7 +2133,7 @@
       <c r="B73" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C73" s="31"/>
+      <c r="C73" s="33"/>
     </row>
     <row r="74" spans="1:3" ht="30">
       <c r="A74" t="s">
@@ -2142,7 +2142,7 @@
       <c r="B74" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="31"/>
+      <c r="C74" s="33"/>
     </row>
     <row r="77" spans="1:3" s="5" customFormat="1" ht="90">
       <c r="B77" s="24" t="s">
@@ -2159,7 +2159,7 @@
       <c r="B79" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C79" s="32" t="s">
+      <c r="C79" s="34" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2170,7 +2170,7 @@
       <c r="B80" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C80" s="32"/>
+      <c r="C80" s="34"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
@@ -2179,7 +2179,7 @@
       <c r="B81" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C81" s="32"/>
+      <c r="C81" s="34"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
@@ -2188,7 +2188,7 @@
       <c r="B82" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C82" s="32"/>
+      <c r="C82" s="34"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
@@ -2197,7 +2197,7 @@
       <c r="B83" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C83" s="32"/>
+      <c r="C83" s="34"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
@@ -2206,7 +2206,7 @@
       <c r="B84" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C84" s="32"/>
+      <c r="C84" s="34"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
@@ -2215,7 +2215,7 @@
       <c r="B85" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C85" s="32"/>
+      <c r="C85" s="34"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
@@ -2224,7 +2224,7 @@
       <c r="B86" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C86" s="32"/>
+      <c r="C86" s="34"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
@@ -2233,7 +2233,7 @@
       <c r="B87" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C87" s="32"/>
+      <c r="C87" s="34"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
@@ -2242,7 +2242,7 @@
       <c r="B88" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C88" s="32"/>
+      <c r="C88" s="34"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
@@ -2251,7 +2251,7 @@
       <c r="B89" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C89" s="32"/>
+      <c r="C89" s="34"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
@@ -2260,7 +2260,7 @@
       <c r="B90" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C90" s="32"/>
+      <c r="C90" s="34"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
@@ -2269,7 +2269,7 @@
       <c r="B91" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C91" s="32"/>
+      <c r="C91" s="34"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
@@ -2278,7 +2278,7 @@
       <c r="B92" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C92" s="32"/>
+      <c r="C92" s="34"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
@@ -2287,7 +2287,7 @@
       <c r="B93" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C93" s="32"/>
+      <c r="C93" s="34"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
@@ -2296,7 +2296,7 @@
       <c r="B94" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C94" s="32"/>
+      <c r="C94" s="34"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
@@ -2305,7 +2305,7 @@
       <c r="B95" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C95" s="32"/>
+      <c r="C95" s="34"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
@@ -2314,7 +2314,7 @@
       <c r="B96" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C96" s="32"/>
+      <c r="C96" s="34"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
@@ -2323,7 +2323,7 @@
       <c r="B97" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C97" s="32"/>
+      <c r="C97" s="34"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
@@ -2332,7 +2332,7 @@
       <c r="B98" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C98" s="32"/>
+      <c r="C98" s="34"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
@@ -2341,7 +2341,7 @@
       <c r="B99" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C99" s="32"/>
+      <c r="C99" s="34"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
@@ -2350,7 +2350,7 @@
       <c r="B100" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C100" s="32"/>
+      <c r="C100" s="34"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
@@ -2359,7 +2359,7 @@
       <c r="B101" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C101" s="32"/>
+      <c r="C101" s="34"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
@@ -2368,7 +2368,7 @@
       <c r="B102" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C102" s="32"/>
+      <c r="C102" s="34"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
@@ -2377,7 +2377,7 @@
       <c r="B103" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C103" s="32"/>
+      <c r="C103" s="34"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
@@ -2386,7 +2386,7 @@
       <c r="B104" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C104" s="32"/>
+      <c r="C104" s="34"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
@@ -2395,7 +2395,7 @@
       <c r="B105" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C105" s="32"/>
+      <c r="C105" s="34"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
@@ -2404,7 +2404,7 @@
       <c r="B106" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="32"/>
+      <c r="C106" s="34"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
@@ -2413,7 +2413,7 @@
       <c r="B107" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C107" s="32"/>
+      <c r="C107" s="34"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
@@ -2422,7 +2422,7 @@
       <c r="B108" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C108" s="32"/>
+      <c r="C108" s="34"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
@@ -2431,7 +2431,7 @@
       <c r="B109" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C109" s="32"/>
+      <c r="C109" s="34"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
@@ -2440,7 +2440,7 @@
       <c r="B110" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C110" s="32"/>
+      <c r="C110" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
minor edit to variable definitions
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.43.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.43.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13350" windowHeight="12090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13356" windowHeight="12096"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Total measured time for the day (1440 minutes for full days)</t>
   </si>
   <si>
-    <t>The total time of sleep outside a bedtime</t>
-  </si>
-  <si>
     <t>Time of walking with a cadence lower than 100</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
   </si>
   <si>
     <t>Whether the  is a work-day or a leisure day. See definitions of number of work and leisure days above. Possible values "Work", "Leisure" or empty</t>
-  </si>
-  <si>
-    <t>Total sleep time within ValidDuration of this calendar day. (both sleep inside and outside bedtime. For SCAPIS only sleep inside bedtime is found)</t>
   </si>
   <si>
     <t>Number of breaks of sitting or lying postures. (i.e. this is the number of times a person rises from a sitting or a lying posture)</t>
@@ -911,6 +905,12 @@
   </si>
   <si>
     <t>ActiPASS Version 1.43 Variable Definitions</t>
+  </si>
+  <si>
+    <t>The total time of sleep outside a bedtime. This variable is renamed as LieStill in versions &gt; 1.50</t>
+  </si>
+  <si>
+    <t>Total sleep time within ValidDuration of this calendar day  (in ProPASS mode only sleep inside bedtime is found).</t>
   </si>
 </sst>
 </file>
@@ -1531,24 +1531,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" customWidth="1"/>
     <col min="2" max="3" width="79" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="30" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:3" s="30" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="2" spans="1:3" ht="15" thickTop="1"/>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -1557,10 +1557,10 @@
         <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30.75" thickTop="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.4" thickTop="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1568,12 +1568,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -1586,12 +1586,12 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="28.8">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -1604,35 +1604,35 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="9" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" ht="30">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" s="19" customFormat="1" ht="60">
+    <row r="12" spans="1:3" s="19" customFormat="1" ht="57.6">
       <c r="B12" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="20"/>
     </row>
@@ -1663,12 +1663,12 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="30">
+    <row r="16" spans="1:3" ht="28.8">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -1694,9 +1694,9 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" s="15" customFormat="1" ht="90">
+    <row r="20" spans="1:3" s="15" customFormat="1" ht="86.4">
       <c r="B20" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20" s="16"/>
     </row>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
       <c r="B22" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -1733,25 +1733,25 @@
         <v>16</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="28.8">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="30">
+    <row r="27" spans="1:3" ht="28.8">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C27" s="4"/>
     </row>
@@ -1760,49 +1760,49 @@
         <v>17</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
       <c r="B29" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" ht="30">
+    <row r="30" spans="1:3" ht="28.8">
       <c r="A30" t="s">
         <v>18</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" s="10"/>
     </row>
-    <row r="31" spans="1:3" ht="90">
+    <row r="31" spans="1:3" ht="86.4">
       <c r="A31" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" s="10"/>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="28.8">
       <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>85</v>
+      <c r="B32" s="10" t="s">
+        <v>199</v>
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="30">
+    <row r="33" spans="1:3" ht="28.8">
       <c r="A33" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="4"/>
     </row>
@@ -1811,12 +1811,12 @@
         <v>22</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
       <c r="B35" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C35" s="6"/>
     </row>
@@ -1825,7 +1825,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -1834,16 +1834,16 @@
         <v>29</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="4"/>
     </row>
@@ -1852,16 +1852,16 @@
         <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="45">
+    <row r="40" spans="1:3" ht="43.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" s="4"/>
     </row>
@@ -1870,7 +1870,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" s="4"/>
     </row>
@@ -1879,7 +1879,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" s="4"/>
     </row>
@@ -1888,7 +1888,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1896,7 +1896,7 @@
         <v>24</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1904,16 +1904,16 @@
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="30">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C46" s="4"/>
     </row>
@@ -1922,7 +1922,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="4"/>
     </row>
@@ -1931,98 +1931,98 @@
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1">
       <c r="C49" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="5" customFormat="1">
       <c r="B50" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="90.75" thickBot="1">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="87" thickBot="1">
       <c r="A51" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B51" s="27" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="43.2">
+      <c r="A53" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B53" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C53" s="29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="28.8">
+      <c r="A54" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="29" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="45">
-      <c r="A53" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="29" t="s">
+    <row r="55" spans="1:3" ht="28.8">
+      <c r="A55" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="28.8">
+      <c r="A56" s="28" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="45">
-      <c r="A54" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="C54" s="29" t="s">
+      <c r="B56" s="29" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="30">
-      <c r="A55" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="30">
-      <c r="A56" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>187</v>
-      </c>
       <c r="C56" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="5" customFormat="1">
       <c r="A57" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="29" t="s">
         <v>188</v>
-      </c>
-      <c r="B57" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1">
@@ -2032,7 +2032,7 @@
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1">
       <c r="B59" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2040,7 +2040,7 @@
         <v>25</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2048,7 +2048,7 @@
         <v>26</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2056,20 +2056,20 @@
         <v>27</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="120">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="100.8">
       <c r="B65" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="C66" s="32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2077,7 +2077,7 @@
         <v>31</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" s="33"/>
     </row>
@@ -2086,7 +2086,7 @@
         <v>32</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C68" s="33"/>
     </row>
@@ -2095,7 +2095,7 @@
         <v>33</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C69" s="33"/>
     </row>
@@ -2104,7 +2104,7 @@
         <v>34</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="33"/>
     </row>
@@ -2113,7 +2113,7 @@
         <v>35</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" s="33"/>
     </row>
@@ -2122,7 +2122,7 @@
         <v>36</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72" s="33"/>
     </row>
@@ -2131,314 +2131,314 @@
         <v>37</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C73" s="33"/>
     </row>
-    <row r="74" spans="1:3" ht="30">
+    <row r="74" spans="1:3" ht="28.8">
       <c r="A74" t="s">
         <v>38</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C74" s="33"/>
     </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="90">
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="72">
       <c r="B77" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C79" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C80" s="34"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C81" s="34"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C82" s="34"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C83" s="34"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C84" s="34"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C85" s="34"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C86" s="34"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C87" s="34"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C88" s="34"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C89" s="34"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C90" s="34"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C91" s="34"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C92" s="34"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C93" s="34"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C94" s="34"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C95" s="34"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C96" s="34"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C97" s="34"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C98" s="34"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C99" s="34"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C100" s="34"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C101" s="34"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C102" s="34"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C103" s="34"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C104" s="34"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C105" s="34"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C106" s="34"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C107" s="34"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C108" s="34"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C109" s="34"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C110" s="34"/>
     </row>

</xml_diff>